<commit_message>
Arena Ex.1 and Ex.2
</commit_message>
<xml_diff>
--- a/model/production/data.xlsx
+++ b/model/production/data.xlsx
@@ -1,32 +1,455 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programming\Data-Science\model\production\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607899C6-9D6F-4F85-A20A-AD6EC7146BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+  <si>
+    <t>工位</t>
+  </si>
+  <si>
+    <t>任务</t>
+  </si>
+  <si>
+    <t>总时间</t>
+  </si>
+  <si>
+    <t>任务时间</t>
+  </si>
+  <si>
+    <t>[1, 17, 5, 2, 3]</t>
+  </si>
+  <si>
+    <t>[29.0, 2.0, 6.0, 3.0, 5.0]</t>
+  </si>
+  <si>
+    <t>[10, 4]</t>
+  </si>
+  <si>
+    <t>[30.0, 22.0]</t>
+  </si>
+  <si>
+    <t>[12, 11]</t>
+  </si>
+  <si>
+    <t>[30.0, 23.0]</t>
+  </si>
+  <si>
+    <t>[6, 8, 7, 9, 14, 18]</t>
+  </si>
+  <si>
+    <t>[14.0, 5.0, 2.0, 22.0, 2.0, 2.0]</t>
+  </si>
+  <si>
+    <t>[13, 15]</t>
+  </si>
+  <si>
+    <t>[23.0, 19.0]</t>
+  </si>
+  <si>
+    <t>[16, 19]</t>
+  </si>
+  <si>
+    <t>[29.0, 19.0]</t>
+  </si>
+  <si>
+    <t>[20, 21, 22, 25]</t>
+  </si>
+  <si>
+    <t>[29.0, 6.0, 10.0, 5.0]</t>
+  </si>
+  <si>
+    <t>[23, 26, 30, 24]</t>
+  </si>
+  <si>
+    <t>[16.0, 5.0, 5.0, 23.0]</t>
+  </si>
+  <si>
+    <t>[27, 31, 28, 34, 32]</t>
+  </si>
+  <si>
+    <t>[5.0, 5.0, 40.0, 2.0, 1.0]</t>
+  </si>
+  <si>
+    <t>[33, 29, 35]</t>
+  </si>
+  <si>
+    <t>[40.0, 2.0, 5.0]</t>
+  </si>
+  <si>
+    <t>闲置时间</t>
+  </si>
+  <si>
+    <t>[6, 10, 7, 8, 14]</t>
+  </si>
+  <si>
+    <t>[12, 15, 18]</t>
+  </si>
+  <si>
+    <t>[19, 16]</t>
+  </si>
+  <si>
+    <t>[20, 4]</t>
+  </si>
+  <si>
+    <t>[21, 9, 11]</t>
+  </si>
+  <si>
+    <t>[22, 13, 25, 30, 26, 31]</t>
+  </si>
+  <si>
+    <t>[23, 32, 24, 27, 34]</t>
+  </si>
+  <si>
+    <t>[33, 35]</t>
+  </si>
+  <si>
+    <t>[28, 29]</t>
+  </si>
+  <si>
+    <t>方法</t>
+  </si>
+  <si>
+    <r>
+      <t>平滑指数</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (SI)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RPW </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>方法</t>
+    </r>
+  </si>
+  <si>
+    <t>莫迪和杨法</t>
+  </si>
+  <si>
+    <t>平衡率</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>排序规则</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>工位数量</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>平滑指数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(SI)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RPW </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>降序</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>任务时间降序</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>后继任务数量降序</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>前驱任务数量降序</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>综合</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RPW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和任务时间</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>选择规则</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最大最小时间工位</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最大时间差工位对</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最大最小闲置时间</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>高于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>低于平均时间</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +460,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,15 +468,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +800,600 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J28" sqref="I24:J28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="29.25" customWidth="1"/>
+    <col min="4" max="4" width="29.4140625" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.58203125" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5">
+        <v>45</v>
+      </c>
+      <c r="I3" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="5">
+        <v>52</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>53</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5">
+        <v>53</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>47</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="5">
+        <v>47</v>
+      </c>
+      <c r="I6" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1">
+        <v>42</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="5">
+        <v>42</v>
+      </c>
+      <c r="I7" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1">
+        <v>48</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="5">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="5">
+        <v>48</v>
+      </c>
+      <c r="I8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="5">
+        <v>7</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="5">
+        <v>50</v>
+      </c>
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1">
+        <v>49</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="5">
+        <v>8</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="5">
+        <v>49</v>
+      </c>
+      <c r="I10" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5">
+        <v>9</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="5">
+        <v>53</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3">
+        <v>47</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="5">
+        <v>10</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="5">
+        <v>47</v>
+      </c>
+      <c r="I12" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45</v>
+      </c>
+      <c r="D17" s="1">
+        <f>53-C17</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1">
+        <v>53</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" ref="D18:D26" si="0">53-C18</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1">
+        <v>51</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="6">
+        <v>19.29</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1">
+        <v>48</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="6">
+        <v>17.55</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1">
+        <v>51</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="1">
+        <v>51</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1">
+        <v>53</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1">
+        <v>47</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="1">
+        <v>45</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="6">
+        <v>10</v>
+      </c>
+      <c r="H25" s="6">
+        <v>17.940000000000001</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="6">
+        <v>17.940000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>10</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3">
+        <v>42</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="6">
+        <v>10</v>
+      </c>
+      <c r="H26" s="6">
+        <v>17.55</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J26" s="6">
+        <v>17.940000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="6">
+        <v>10</v>
+      </c>
+      <c r="H27" s="6">
+        <v>17.940000000000001</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="6">
+        <v>17.940000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="6">
+        <v>10</v>
+      </c>
+      <c r="H28" s="6">
+        <v>16.73</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J28" s="6">
+        <v>17.940000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="6">
+        <v>10</v>
+      </c>
+      <c r="H29" s="6">
+        <v>17.940000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>